<commit_message>
forgot to push hash file addition
</commit_message>
<xml_diff>
--- a/functions/input.xlsx
+++ b/functions/input.xlsx
@@ -1,42 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ork\LightHouse\Assignment\Maximize\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elad.ron\OneDrive - Technion\Technion\Semester 8\Yearly Project\LightHouse\Assignment\Maximize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EFEB71-270F-4ABD-B162-C3BD5668793D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{A5C86AB3-7C21-4EAF-A2B5-F172B8BD8ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7B4F987-5C1B-4379-9A04-F9A6F8007660}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+  <si>
+    <t>ברגים</t>
+  </si>
   <si>
     <t>בוכנה</t>
   </si>
@@ -47,49 +39,34 @@
     <t>מים</t>
   </si>
   <si>
-    <t>ברגים</t>
-  </si>
-  <si>
     <t>שם תחנה</t>
   </si>
   <si>
+    <t>מספר תחנה</t>
+  </si>
+  <si>
+    <t>כמות עמדות מתחנה</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
     <t>האם מגיע?</t>
-  </si>
-  <si>
-    <t>מספר תחנה</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>כמות עמדות מתחנה</t>
-  </si>
-  <si>
-    <t>253</t>
-  </si>
-  <si>
-    <t>אור</t>
-  </si>
-  <si>
-    <t>אלעד</t>
   </si>
 </sst>
 </file>
@@ -154,8 +131,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,41 +532,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -602,12 +579,12 @@
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -619,19 +596,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F3" s="8">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -643,17 +616,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F4" s="8">
-        <v>60</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -667,17 +636,14 @@
         <v>9</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F5" s="8">
-        <v>60</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -687,21 +653,17 @@
       <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9">
-        <v>80</v>
+      <c r="D6" s="8">
+        <v>400</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F6" s="8">
-        <v>100</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -711,21 +673,17 @@
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="9">
-        <v>80</v>
+      <c r="D7" s="8">
+        <v>200</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F7" s="8">
-        <v>100</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -739,17 +697,14 @@
         <v>7</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F8" s="8">
-        <v>60</v>
-      </c>
-      <c r="G8" s="7"/>
+        <v>300</v>
+      </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -759,45 +714,37 @@
       <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9">
-        <v>400</v>
+      <c r="D9" s="8">
+        <v>2000</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F9" s="8">
-        <v>240</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="9">
-        <v>120</v>
-      </c>
-      <c r="D10" s="9">
-        <v>200</v>
-      </c>
-      <c r="E10" s="9">
-        <v>400</v>
+      <c r="C10" s="8">
+        <v>600</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2000</v>
       </c>
       <c r="F10" s="8">
-        <v>200</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -811,42 +758,33 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F11" s="8">
-        <v>200</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="9">
-        <v>280</v>
-      </c>
-      <c r="D12" s="9">
-        <v>200</v>
-      </c>
-      <c r="E12" s="9">
-        <v>160</v>
+      <c r="C12" s="8">
+        <v>1300</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="8">
+        <v>800</v>
       </c>
       <c r="F12" s="8">
-        <v>240</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -860,41 +798,33 @@
         <v>9</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F13" s="8">
-        <v>100</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="9">
-        <v>140</v>
-      </c>
-      <c r="D14" s="9">
-        <v>200</v>
+      <c r="C14" s="8">
+        <v>700</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1000</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F14" s="8">
-        <v>200</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -905,20 +835,16 @@
         <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="9">
-        <v>160</v>
+        <v>9</v>
+      </c>
+      <c r="E15" s="8">
+        <v>800</v>
       </c>
       <c r="F15" s="8">
-        <v>120</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -932,17 +858,13 @@
         <v>7</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F16" s="8">
-        <v>160</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -956,17 +878,13 @@
         <v>10</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F17" s="8">
-        <v>120</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -979,42 +897,34 @@
       <c r="D18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="9">
-        <v>300</v>
+      <c r="E18" s="8">
+        <v>1500</v>
       </c>
       <c r="F18" s="8">
-        <v>100</v>
-      </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="9">
-        <v>160</v>
+      <c r="C19" s="8">
+        <v>800</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F19" s="8">
-        <v>120</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1025,44 +935,36 @@
         <v>7</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="9">
-        <v>300</v>
+        <v>9</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1500</v>
       </c>
       <c r="F20" s="8">
-        <v>120</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="9">
-        <v>160</v>
+      <c r="C21" s="8">
+        <v>800</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" s="8">
-        <v>160</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1072,23 +974,18 @@
       <c r="C22" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="9">
-        <v>100</v>
+      <c r="D22" s="8">
+        <v>500</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F22" s="8">
-        <v>100</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
       <c r="C23" s="4">
         <v>3</v>
       </c>
@@ -1102,7 +999,7 @@
         <v>11</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1110,4 +1007,245 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100798944B7ACF28E41AA1150A249DECACE" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb6014ec5bdbea0aa9dfe7b393ae331c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="13fdcbf6-4821-45fd-ada2-95945239b561" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f1495b93262afdd3f650199dcde1e76" ns3:_="">
+    <xsd:import namespace="13fdcbf6-4821-45fd-ada2-95945239b561"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="13fdcbf6-4821-45fd-ada2-95945239b561" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5EA9329-F84B-4C8A-B24A-80A0885395E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="13fdcbf6-4821-45fd-ada2-95945239b561"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4F36981-3B81-461B-9DAB-5F60E01D98A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{562FD7E7-9DE5-4568-B12A-6198740C5563}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="13fdcbf6-4821-45fd-ada2-95945239b561"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>